<commit_message>
dispatch suite & order creation optimization
</commit_message>
<xml_diff>
--- a/3.0/src/test/java/data/DataSheet.xlsx
+++ b/3.0/src/test/java/data/DataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" state="visible" r:id="rId3"/>
@@ -47,10 +47,10 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">2ss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7ss</t>
+    <t xml:space="preserve">2SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7SS</t>
   </si>
 </sst>
 </file>
@@ -291,7 +291,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -342,7 +342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -365,8 +365,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>